<commit_message>
added test data, some more work on tests and pages methods
</commit_message>
<xml_diff>
--- a/excel/test_data.xlsx
+++ b/excel/test_data.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZ\edureka_pom_automation\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A408F9B6-7723-4C08-9B47-5374CDB98EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD9CA39-4893-4520-BDD2-2A95CDBFABA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{593A2C51-7F2B-432B-B81B-9F914E97F10A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{593A2C51-7F2B-432B-B81B-9F914E97F10A}"/>
   </bookViews>
   <sheets>
     <sheet name="register_data" sheetId="1" r:id="rId1"/>
     <sheet name="login_data" sheetId="2" r:id="rId2"/>
+    <sheet name="login_data_fail" sheetId="3" r:id="rId3"/>
+    <sheet name="register_data_fail" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,12 +27,101 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phoneno</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>asdretu@gmail.com</t>
+  </si>
+  <si>
+    <t>Asedased</t>
+  </si>
+  <si>
+    <t>fdgfdgdsfgdsf</t>
+  </si>
+  <si>
+    <t>asdretsdu@gmail.com</t>
+  </si>
+  <si>
+    <t>adsed</t>
+  </si>
+  <si>
+    <t>Asedasedfgf</t>
+  </si>
+  <si>
+    <t>cvbcvbcvb</t>
+  </si>
+  <si>
+    <t>bcvbcv</t>
+  </si>
+  <si>
+    <t>AsedasedasAsedasedasAsedasedasAsedasedasAsedasedass</t>
+  </si>
+  <si>
+    <t>asdretdu@gmail.com</t>
+  </si>
+  <si>
+    <t>ASEDSAFR</t>
+  </si>
+  <si>
+    <t>asedased</t>
+  </si>
+  <si>
+    <t>As</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t>#$%&amp;/()=</t>
+  </si>
+  <si>
+    <t>gdgdgsdgd</t>
+  </si>
+  <si>
+    <t>fdsfdsffsd</t>
+  </si>
+  <si>
+    <t>sdfsdfdsf</t>
+  </si>
+  <si>
+    <t>fsdfsdfsdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                           </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -54,13 +145,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -365,7 +460,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -373,28 +468,363 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1B5EFD-506A-4221-9B18-BFE452B69362}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>658987542</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{47CB370A-AD09-4488-81D3-2E390355C8DA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AB0872-326C-4592-9415-A9FE8D7038EA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{2E636749-5A39-4A09-B17A-93B9BFB18128}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA363617-B560-4EE1-B36B-D744B4745992}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{9A6B84A9-E153-4CFD-913E-438374D728FF}"/>
+    <hyperlink ref="A6" r:id="rId2" xr:uid="{C8681B1E-044A-4F14-9E66-DD50ECAC6A20}"/>
+    <hyperlink ref="A7" r:id="rId3" xr:uid="{FAE4DFF2-F3F5-4AAA-9429-48C2344B120C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9468E4-C586-415B-8842-BB6A3A40B958}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>658987542</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>658986542</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>658987542</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>658987542</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>658987542</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>658987542</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>658987542</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>658987542</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>658987542</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>658987542</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2">
+        <v>6.5898755426589801E+79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>658987542</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{89900C63-2A1E-4611-B3A1-92E772EDCDD9}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{36CC9AB2-5F5D-462E-8F96-8352CA815275}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{220B67D9-F768-4BBD-815E-870334BC6884}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{D6003248-9AC9-49E5-B19C-0430A75A3E8A}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{24460DA1-19D7-4075-927C-73B448988718}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{272E3DDC-EAAD-409B-A290-AF10249E6AE3}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{DBC16053-3AFB-4F41-8871-FF54F0FA2ED0}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{61913C3F-0D9F-449A-992A-7E214A23FAB6}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{4A1EC02A-9477-422B-B14C-63B9F535A7D1}"/>
+    <hyperlink ref="A13" r:id="rId10" xr:uid="{EA18A86E-87E2-480C-BCC5-216E99C0685B}"/>
+    <hyperlink ref="A16" r:id="rId11" xr:uid="{AF5E2077-90D6-4ECE-8658-5921BBCC575E}"/>
+    <hyperlink ref="A17" r:id="rId12" xr:uid="{110462FD-6090-4A84-9787-124E4DB0E3EE}"/>
+    <hyperlink ref="A19" r:id="rId13" xr:uid="{78A6B7FA-F952-4F22-8661-0E07077925FA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added decorators, fixed tests, added some more base page methods
</commit_message>
<xml_diff>
--- a/excel/test_data.xlsx
+++ b/excel/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZ\edureka_pom_automation\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD9CA39-4893-4520-BDD2-2A95CDBFABA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE3892C-FC7A-4A9D-8BBD-6F54C5C54671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{593A2C51-7F2B-432B-B81B-9F914E97F10A}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>email</t>
   </si>
@@ -54,9 +54,6 @@
     <t>adsed</t>
   </si>
   <si>
-    <t>Asedasedfgf</t>
-  </si>
-  <si>
     <t>cvbcvbcvb</t>
   </si>
   <si>
@@ -103,6 +100,18 @@
   </si>
   <si>
     <t xml:space="preserve">                           </t>
+  </si>
+  <si>
+    <t>asdhfgretu@gmail.com</t>
+  </si>
+  <si>
+    <t>afghsdretu@gmail.com</t>
+  </si>
+  <si>
+    <t>rekuhzdftu@gmail.com</t>
+  </si>
+  <si>
+    <t>Asedasedfgfghfghgf</t>
   </si>
 </sst>
 </file>
@@ -471,12 +480,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
   </cols>
@@ -494,7 +503,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>658987542</v>
@@ -554,7 +563,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,15 +611,15 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -628,7 +637,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD35"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +660,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>658987542</v>
@@ -662,51 +671,51 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>658986542</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>658987542</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>658987542</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>658987542</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>658987542</v>
@@ -714,29 +723,29 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>658987542</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>658987542</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -746,7 +755,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>42</v>
@@ -754,7 +763,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>658987542</v>
@@ -762,23 +771,23 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
         <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2">
         <v>6.5898755426589801E+79</v>
@@ -786,7 +795,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>658987542</v>
@@ -794,18 +803,18 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -813,18 +822,12 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{89900C63-2A1E-4611-B3A1-92E772EDCDD9}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{36CC9AB2-5F5D-462E-8F96-8352CA815275}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{220B67D9-F768-4BBD-815E-870334BC6884}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{D6003248-9AC9-49E5-B19C-0430A75A3E8A}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{24460DA1-19D7-4075-927C-73B448988718}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{272E3DDC-EAAD-409B-A290-AF10249E6AE3}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{DBC16053-3AFB-4F41-8871-FF54F0FA2ED0}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{61913C3F-0D9F-449A-992A-7E214A23FAB6}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{4A1EC02A-9477-422B-B14C-63B9F535A7D1}"/>
-    <hyperlink ref="A13" r:id="rId10" xr:uid="{EA18A86E-87E2-480C-BCC5-216E99C0685B}"/>
-    <hyperlink ref="A16" r:id="rId11" xr:uid="{AF5E2077-90D6-4ECE-8658-5921BBCC575E}"/>
-    <hyperlink ref="A17" r:id="rId12" xr:uid="{110462FD-6090-4A84-9787-124E4DB0E3EE}"/>
-    <hyperlink ref="A19" r:id="rId13" xr:uid="{78A6B7FA-F952-4F22-8661-0E07077925FA}"/>
+    <hyperlink ref="A5:A10" r:id="rId4" display="afghsdretu@gmail.com" xr:uid="{B27A7AA5-9BF6-421E-9E3F-A4706E7D64D2}"/>
+    <hyperlink ref="A13" r:id="rId5" xr:uid="{723CD613-A8F3-4D2E-867A-53509A25811A}"/>
+    <hyperlink ref="A16:A17" r:id="rId6" display="afghsdretu@gmail.com" xr:uid="{2FBE539E-86D9-418E-A5DF-D45EECEDC716}"/>
+    <hyperlink ref="A19" r:id="rId7" xr:uid="{4BE9A3D9-637A-4BB3-AF57-B67EA2FDC163}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>